<commit_message>
Remove old uml version, work on prse d'avis.
</commit_message>
<xml_diff>
--- a/timeline_exemple.xlsx
+++ b/timeline_exemple.xlsx
@@ -121,7 +121,7 @@
   <dimension ref="A2:AM8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -453,9 +453,7 @@
   <printOptions/>
   <pageMargins left="1" right="1" top="1.667" bottom="1.667" header="1" footer="1"/>
   <pageSetup/>
-  <rowBreaks count="1">
-    <brk id="32" max="16383"/>
-  </rowBreaks>
+  <rowBreaks count="0"/>
   <colBreaks count="0"/>
 </worksheet>
 </file>

</xml_diff>